<commit_message>
Fixed data files for upper age = 20
</commit_message>
<xml_diff>
--- a/data/hake_intrasp_221011.xlsx
+++ b/data/hake_intrasp_221011.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BFFA23-5459-354D-BE98-825AC795CCDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A199C53A-0C5F-7747-8527-DA616762A199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="42700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="42700" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -17750,7 +17750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
+    <sheetView zoomScale="175" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -40861,8 +40861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:DR21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W28" sqref="W28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U42" sqref="U42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -41252,28 +41252,28 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.96</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>0.84210526315789502</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>0.39583333333333298</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>0.19512195121951201</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>1.7857142857142901E-2</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>1.0989010989011E-2</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -41623,37 +41623,37 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>0.157894736842105</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>0.60416666666666696</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>0.80487804878048796</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>0.89285714285714302</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>0.80219780219780201</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>0.52586206896551702</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>0.196850393700787</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>4.3062200956937802E-2</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>2.9032258064516099E-2</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -42006,31 +42006,31 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>8.9285714285714302E-2</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>0.164835164835165</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>0.45689655172413801</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>0.71653543307086598</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>0.57416267942583699</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>0.19354838709677399</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>4.8109965635738799E-2</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>2.95566502463054E-2</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>1.0989010989011E-2</v>
       </c>
       <c r="U4">
         <v>0</v>
@@ -42377,31 +42377,31 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>1.0989010989011E-2</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>8.6206896551724102E-3</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>5.5118110236220499E-2</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>0.22966507177033499</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>0.43225806451612903</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>0.34020618556700999</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>0.201970443349754</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>8.7912087912087905E-2</v>
       </c>
       <c r="U5">
-        <v>0</v>
+        <v>2.2222222222222199E-2</v>
       </c>
       <c r="V5">
         <v>0</v>
@@ -42745,37 +42745,37 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>1.0989010989011E-2</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>8.6206896551724102E-3</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>2.3622047244094498E-2</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>0.119617224880383</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>0.261290322580645</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>0.34364261168384902</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <v>0.31527093596059103</v>
       </c>
       <c r="T6">
-        <v>0</v>
+        <v>0.19780219780219799</v>
       </c>
       <c r="U6">
-        <v>0</v>
+        <v>7.7777777777777807E-2</v>
       </c>
       <c r="V6">
-        <v>0</v>
+        <v>3.6363636363636397E-2</v>
       </c>
       <c r="W6">
-        <v>0</v>
+        <v>2.0833333333333301E-2</v>
       </c>
       <c r="X6">
         <v>0</v>
@@ -43122,43 +43122,43 @@
         <v>0</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>3.3492822966507199E-2</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <v>7.7419354838709695E-2</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>0.240549828178694</v>
       </c>
       <c r="S7">
-        <v>0</v>
+        <v>0.31034482758620702</v>
       </c>
       <c r="T7">
-        <v>0</v>
+        <v>0.230769230769231</v>
       </c>
       <c r="U7">
-        <v>0</v>
+        <v>0.22222222222222199</v>
       </c>
       <c r="V7">
-        <v>0</v>
+        <v>0.109090909090909</v>
       </c>
       <c r="W7">
-        <v>0</v>
+        <v>8.3333333333333301E-2</v>
       </c>
       <c r="X7">
-        <v>0</v>
+        <v>0.114285714285714</v>
       </c>
       <c r="Y7">
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="Z7">
-        <v>0</v>
+        <v>0.266666666666667</v>
       </c>
       <c r="AA7">
-        <v>0</v>
+        <v>0.1875</v>
       </c>
       <c r="AB7">
-        <v>0</v>
+        <v>9.0909090909090898E-2</v>
       </c>
       <c r="AC7">
         <v>0</v>
@@ -43487,55 +43487,55 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <v>7.8740157480314994E-3</v>
       </c>
       <c r="P8">
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>0</v>
+        <v>6.4516129032258099E-3</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>2.06185567010309E-2</v>
       </c>
       <c r="S8">
-        <v>0</v>
+        <v>4.4334975369458102E-2</v>
       </c>
       <c r="T8">
-        <v>0</v>
+        <v>0.14285714285714299</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <v>0.16666666666666699</v>
       </c>
       <c r="V8">
-        <v>0</v>
+        <v>0.27272727272727298</v>
       </c>
       <c r="W8">
-        <v>0</v>
+        <v>8.3333333333333301E-2</v>
       </c>
       <c r="X8">
-        <v>0</v>
+        <v>0.14285714285714299</v>
       </c>
       <c r="Y8">
-        <v>0</v>
+        <v>0.15625</v>
       </c>
       <c r="Z8">
-        <v>0</v>
+        <v>6.6666666666666693E-2</v>
       </c>
       <c r="AA8">
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="AB8">
-        <v>0</v>
+        <v>9.0909090909090898E-2</v>
       </c>
       <c r="AC8">
-        <v>0</v>
+        <v>0.16666666666666699</v>
       </c>
       <c r="AD8">
-        <v>0</v>
+        <v>0.14285714285714299</v>
       </c>
       <c r="AE8">
-        <v>0</v>
+        <v>9.0909090909090898E-2</v>
       </c>
       <c r="AF8">
         <v>0</v>
@@ -43864,43 +43864,43 @@
         <v>0</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>3.4364261168384901E-3</v>
       </c>
       <c r="S9">
-        <v>0</v>
+        <v>4.9261083743842402E-2</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <v>0.15384615384615399</v>
       </c>
       <c r="U9">
-        <v>0</v>
+        <v>0.17777777777777801</v>
       </c>
       <c r="V9">
-        <v>0</v>
+        <v>0.12727272727272701</v>
       </c>
       <c r="W9">
-        <v>0</v>
+        <v>0.104166666666667</v>
       </c>
       <c r="X9">
-        <v>0</v>
+        <v>8.5714285714285701E-2</v>
       </c>
       <c r="Y9">
-        <v>0</v>
+        <v>0.15625</v>
       </c>
       <c r="Z9">
-        <v>0</v>
+        <v>0.266666666666667</v>
       </c>
       <c r="AA9">
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="AB9">
-        <v>0</v>
+        <v>9.0909090909090898E-2</v>
       </c>
       <c r="AC9">
-        <v>0</v>
+        <v>8.3333333333333301E-2</v>
       </c>
       <c r="AD9">
-        <v>0</v>
+        <v>0.42857142857142899</v>
       </c>
       <c r="AE9">
         <v>0</v>
@@ -44232,46 +44232,46 @@
         <v>0</v>
       </c>
       <c r="R10">
-        <v>0</v>
+        <v>3.4364261168384901E-3</v>
       </c>
       <c r="S10">
-        <v>0</v>
+        <v>1.9704433497536901E-2</v>
       </c>
       <c r="T10">
-        <v>0</v>
+        <v>5.4945054945054903E-2</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>6.6666666666666693E-2</v>
       </c>
       <c r="V10">
-        <v>0</v>
+        <v>3.6363636363636397E-2</v>
       </c>
       <c r="W10">
-        <v>0</v>
+        <v>0.14583333333333301</v>
       </c>
       <c r="X10">
-        <v>0</v>
+        <v>5.7142857142857099E-2</v>
       </c>
       <c r="Y10">
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
       <c r="Z10">
         <v>0</v>
       </c>
       <c r="AA10">
-        <v>0</v>
+        <v>0.1875</v>
       </c>
       <c r="AB10">
-        <v>0</v>
+        <v>0.18181818181818199</v>
       </c>
       <c r="AC10">
-        <v>0</v>
+        <v>0.16666666666666699</v>
       </c>
       <c r="AD10">
         <v>0</v>
       </c>
       <c r="AE10">
-        <v>0</v>
+        <v>0.18181818181818199</v>
       </c>
       <c r="AF10">
         <v>0</v>
@@ -44603,43 +44603,43 @@
         <v>0</v>
       </c>
       <c r="S11">
-        <v>0</v>
+        <v>1.47783251231527E-2</v>
       </c>
       <c r="T11">
-        <v>0</v>
+        <v>5.4945054945054903E-2</v>
       </c>
       <c r="U11">
-        <v>0</v>
+        <v>8.8888888888888906E-2</v>
       </c>
       <c r="V11">
-        <v>0</v>
+        <v>0.109090909090909</v>
       </c>
       <c r="W11">
-        <v>0</v>
+        <v>0.104166666666667</v>
       </c>
       <c r="X11">
-        <v>0</v>
+        <v>0.114285714285714</v>
       </c>
       <c r="Y11">
-        <v>0</v>
+        <v>0.1875</v>
       </c>
       <c r="Z11">
-        <v>0</v>
+        <v>6.6666666666666693E-2</v>
       </c>
       <c r="AA11">
-        <v>0</v>
+        <v>0.1875</v>
       </c>
       <c r="AB11">
-        <v>0</v>
+        <v>0.36363636363636398</v>
       </c>
       <c r="AC11">
-        <v>0</v>
+        <v>0.16666666666666699</v>
       </c>
       <c r="AD11">
-        <v>0</v>
+        <v>0.28571428571428598</v>
       </c>
       <c r="AE11">
-        <v>0</v>
+        <v>0.36363636363636398</v>
       </c>
       <c r="AF11">
         <v>0</v>
@@ -44971,43 +44971,43 @@
         <v>0</v>
       </c>
       <c r="S12">
-        <v>0</v>
+        <v>4.92610837438424E-3</v>
       </c>
       <c r="T12">
-        <v>0</v>
+        <v>3.2967032967033003E-2</v>
       </c>
       <c r="U12">
-        <v>0</v>
+        <v>4.4444444444444398E-2</v>
       </c>
       <c r="V12">
-        <v>0</v>
+        <v>5.4545454545454501E-2</v>
       </c>
       <c r="W12">
-        <v>0</v>
+        <v>0.104166666666667</v>
       </c>
       <c r="X12">
-        <v>0</v>
+        <v>8.5714285714285701E-2</v>
       </c>
       <c r="Y12">
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
       <c r="Z12">
-        <v>0</v>
+        <v>6.6666666666666693E-2</v>
       </c>
       <c r="AA12">
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="AB12">
         <v>0</v>
       </c>
       <c r="AC12">
-        <v>0</v>
+        <v>8.3333333333333301E-2</v>
       </c>
       <c r="AD12">
         <v>0</v>
       </c>
       <c r="AE12">
-        <v>0</v>
+        <v>0.27272727272727298</v>
       </c>
     </row>
     <row r="13" spans="1:122" x14ac:dyDescent="0.2">
@@ -45066,28 +45066,28 @@
         <v>0</v>
       </c>
       <c r="S13">
-        <v>0</v>
+        <v>9.8522167487684695E-3</v>
       </c>
       <c r="T13">
         <v>0</v>
       </c>
       <c r="U13">
-        <v>0</v>
+        <v>3.3333333333333298E-2</v>
       </c>
       <c r="V13">
-        <v>0</v>
+        <v>3.6363636363636397E-2</v>
       </c>
       <c r="W13">
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="X13">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="Y13">
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="Z13">
-        <v>0</v>
+        <v>6.6666666666666693E-2</v>
       </c>
       <c r="AA13">
         <v>0</v>
@@ -45102,7 +45102,7 @@
         <v>0</v>
       </c>
       <c r="AE13">
-        <v>0</v>
+        <v>9.0909090909090898E-2</v>
       </c>
     </row>
     <row r="14" spans="1:122" x14ac:dyDescent="0.2">
@@ -45167,31 +45167,31 @@
         <v>0</v>
       </c>
       <c r="U14">
-        <v>0</v>
+        <v>6.6666666666666693E-2</v>
       </c>
       <c r="V14">
-        <v>0</v>
+        <v>0.109090909090909</v>
       </c>
       <c r="W14">
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="X14">
-        <v>0</v>
+        <v>2.8571428571428598E-2</v>
       </c>
       <c r="Y14">
-        <v>0</v>
+        <v>0.15625</v>
       </c>
       <c r="Z14">
         <v>0</v>
       </c>
       <c r="AA14">
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="AB14">
         <v>0</v>
       </c>
       <c r="AC14">
-        <v>0</v>
+        <v>0.16666666666666699</v>
       </c>
       <c r="AD14">
         <v>0</v>
@@ -45262,25 +45262,25 @@
         <v>0</v>
       </c>
       <c r="U15">
-        <v>0</v>
+        <v>3.3333333333333298E-2</v>
       </c>
       <c r="V15">
-        <v>0</v>
+        <v>7.2727272727272696E-2</v>
       </c>
       <c r="W15">
-        <v>0</v>
+        <v>0.104166666666667</v>
       </c>
       <c r="X15">
-        <v>0</v>
+        <v>0.14285714285714299</v>
       </c>
       <c r="Y15">
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="Z15">
-        <v>0</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="AA15">
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="AB15">
         <v>0</v>
@@ -45289,7 +45289,7 @@
         <v>0</v>
       </c>
       <c r="AD15">
-        <v>0</v>
+        <v>0.14285714285714299</v>
       </c>
       <c r="AE15">
         <v>0</v>
@@ -45354,34 +45354,34 @@
         <v>0</v>
       </c>
       <c r="T16">
-        <v>0</v>
+        <v>2.1978021978022001E-2</v>
       </c>
       <c r="U16">
         <v>0</v>
       </c>
       <c r="V16">
-        <v>0</v>
+        <v>1.8181818181818198E-2</v>
       </c>
       <c r="W16">
-        <v>0</v>
+        <v>2.0833333333333301E-2</v>
       </c>
       <c r="X16">
         <v>0</v>
       </c>
       <c r="Y16">
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
       <c r="Z16">
-        <v>0</v>
+        <v>6.6666666666666693E-2</v>
       </c>
       <c r="AA16">
         <v>0</v>
       </c>
       <c r="AB16">
-        <v>0</v>
+        <v>9.0909090909090898E-2</v>
       </c>
       <c r="AC16">
-        <v>0</v>
+        <v>8.3333333333333301E-2</v>
       </c>
       <c r="AD16">
         <v>0</v>
@@ -45449,22 +45449,22 @@
         <v>0</v>
       </c>
       <c r="T17">
-        <v>0</v>
+        <v>1.0989010989011E-2</v>
       </c>
       <c r="U17">
         <v>0</v>
       </c>
       <c r="V17">
-        <v>0</v>
+        <v>1.8181818181818198E-2</v>
       </c>
       <c r="W17">
-        <v>0</v>
+        <v>4.1666666666666699E-2</v>
       </c>
       <c r="X17">
-        <v>0</v>
+        <v>2.8571428571428598E-2</v>
       </c>
       <c r="Y17">
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="Z17">
         <v>0</v>
@@ -45473,10 +45473,10 @@
         <v>0</v>
       </c>
       <c r="AB17">
-        <v>0</v>
+        <v>9.0909090909090898E-2</v>
       </c>
       <c r="AC17">
-        <v>0</v>
+        <v>8.3333333333333301E-2</v>
       </c>
       <c r="AD17">
         <v>0</v>
@@ -45554,7 +45554,7 @@
         <v>0</v>
       </c>
       <c r="W18">
-        <v>0</v>
+        <v>4.1666666666666699E-2</v>
       </c>
       <c r="X18">
         <v>0</v>
@@ -45650,7 +45650,7 @@
         <v>0</v>
       </c>
       <c r="W19">
-        <v>0</v>
+        <v>2.0833333333333301E-2</v>
       </c>
       <c r="X19">
         <v>0</v>

</xml_diff>

<commit_message>
Updated & renamed CEATTLE data input files
</commit_message>
<xml_diff>
--- a/data/hake_intrasp_221011.xlsx
+++ b/data/hake_intrasp_221011.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9183AE72-E1EB-C748-8D93-0776C378CC46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675D70D1-2345-B34B-A84B-EE6AC1627117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21760" yWindow="500" windowWidth="38400" windowHeight="33340" firstSheet="1" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7480" yWindow="500" windowWidth="30080" windowHeight="33340" firstSheet="1" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -2878,7 +2878,7 @@
   <dimension ref="A1:AF21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R31" sqref="R31"/>
+      <selection activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4338,7 +4338,7 @@
         <v>0</v>
       </c>
       <c r="V21">
-        <v>1.8633999999999999</v>
+        <v>3.3879999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -14032,8 +14032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Z107" sqref="Z107"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14144,64 +14144,64 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="D2">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="E2">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="F2">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="G2">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="H2">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="I2">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="J2">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="K2">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="L2">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="M2">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="N2">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="O2">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="P2">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="Q2">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="R2">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="S2">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="T2">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="U2">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="V2">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>
@@ -17932,7 +17932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O62" sqref="O62"/>
     </sheetView>
   </sheetViews>

</xml_diff>